<commit_message>
updated test cases Nov16
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/Test_Data_Sheet.xlsx
+++ b/target/test-classes/testdata/Test_Data_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\eclipse-workspace\Regression_Pos_project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753B04F3-02D1-4C7C-9147-0ADB4A6465B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180DF5D0-E5A3-4028-8D71-FE8463B70EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="751" activeTab="2" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
   </bookViews>
@@ -1880,7 +1880,7 @@
     <t>Single Product Test Case</t>
   </si>
   <si>
-    <t>212222</t>
+    <t>212223</t>
   </si>
 </sst>
 </file>
@@ -3368,7 +3368,7 @@
   <dimension ref="A2:AI54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>